<commit_message>
faker module pushed to git
</commit_message>
<xml_diff>
--- a/Deepesh/PythonProgramming/Python_Modules/users_details.xlsx
+++ b/Deepesh/PythonProgramming/Python_Modules/users_details.xlsx
@@ -424,1078 +424,1078 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>James</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>michael74@example.org</t>
+          <t>jessica84@example.org</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>(410)312-4471x8199</t>
+          <t>253.302.7370</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Robin</t>
+          <t>William</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Wilkinson</t>
+          <t>Roth</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>wongkyle@example.org</t>
+          <t>billy12@example.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(528)856-9122x8694</t>
+          <t>873-841-3042x60978</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Walter</t>
+          <t>Roy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Merritt</t>
+          <t>Lyons</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>lindseywhite@example.net</t>
+          <t>monica41@example.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6367628014</t>
+          <t>4085959353</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sexton</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>kristalandry@example.com</t>
+          <t>akennedy@example.org</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>930.814.2623</t>
+          <t>384-701-4754</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gregory</t>
+          <t>Christine</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>joshua21@example.com</t>
+          <t>bhodges@example.net</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+1-532-907-8731x51481</t>
+          <t>001-868-696-3107x56462</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Campbell</t>
+          <t>Gardner</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>wjohnson@example.com</t>
+          <t>sherryprice@example.org</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>217.389.0374x9189</t>
+          <t>821-226-3604</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tiffany</t>
+          <t>Timothy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t>Perez</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>wsawyer@example.com</t>
+          <t>danielfoster@example.org</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>350-662-4028x7915</t>
+          <t>759.785.4635</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Whitney</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Stevens</t>
+          <t>Martinez</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>allen37@example.com</t>
+          <t>seansanchez@example.net</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>(425)840-3878</t>
+          <t>315.704.4982x7779</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kyle</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Roberts</t>
+          <t>Castillo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>thomasmcfarland@example.com</t>
+          <t>wwalker@example.org</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5053264713</t>
+          <t>(961)298-0738x92660</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Sharon</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hill</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>sandra63@example.org</t>
+          <t>vphillips@example.net</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>752-568-0873x19326</t>
+          <t>9189362930</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>Mia</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Liu</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>shannonsimmons@example.org</t>
+          <t>greenemaria@example.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>434.643.5571x59051</t>
+          <t>(830)928-9081</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Todd</t>
+          <t>David</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rivera</t>
+          <t>Downs</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>scottdaniel@example.com</t>
+          <t>dgordon@example.org</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>(894)494-5371x309</t>
+          <t>+1-903-513-8724x6346</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Rickey</t>
+          <t>Brandy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cain</t>
+          <t>White</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>gclark@example.net</t>
+          <t>kbenson@example.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>+1-470-601-8342x4070</t>
+          <t>4184204038</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Michelle</t>
+          <t>Jennifer</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Phillips</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lisarosario@example.com</t>
+          <t>ysmith@example.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>(921)368-7341x2457</t>
+          <t>+1-979-482-8665x201</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kayla</t>
+          <t>Amy</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Walker</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>veronica17@example.net</t>
+          <t>calebpowell@example.com</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>+1-679-514-3460x816</t>
+          <t>+1-479-445-3207x5997</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tyler</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Coleman</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>jon28@example.com</t>
+          <t>adam35@example.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>725-433-8360x0405</t>
+          <t>001-303-830-1826x617</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Cynthia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Weaver</t>
+          <t>Freeman</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>inichols@example.org</t>
+          <t>kevinsharp@example.org</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>(438)623-8328x34090</t>
+          <t>+1-639-851-0189x756</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Joshua</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ray</t>
+          <t>May</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>karenknox@example.net</t>
+          <t>kirsten47@example.net</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>355-898-8498x5816</t>
+          <t>(848)705-3659x100</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Heidi</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Swanson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>daviswhitney@example.com</t>
+          <t>jimmy04@example.org</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>(510)328-0501x35293</t>
+          <t>471-669-3904</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Oconnell</t>
+          <t>Francis</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>william67@example.org</t>
+          <t>michael26@example.net</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>001-979-987-5308x520</t>
+          <t>335-426-7572</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Kathleen</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Parker</t>
+          <t>Barnes</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>akeller@example.com</t>
+          <t>jordanchelsea@example.com</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>636.996.8602</t>
+          <t>+1-976-854-0346x6336</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Hurst</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>johnsonmegan@example.org</t>
+          <t>marklandry@example.net</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>(474)975-5510x3252</t>
+          <t>804.494.4234x10343</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Castro</t>
+          <t>Odonnell</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>sthompson@example.com</t>
+          <t>kevin43@example.org</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>+1-872-922-0389</t>
+          <t>329.608.5203x82743</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Erica</t>
+          <t>Yolanda</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Keller</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>whitelorraine@example.org</t>
+          <t>mary86@example.org</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>+1-211-623-1389x81724</t>
+          <t>521-769-7755</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Nathan</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Alvarado</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>barnesrebecca@example.com</t>
+          <t>toniwright@example.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>887.895.5308</t>
+          <t>859.879.3812</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Goodman</t>
+          <t>King</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>newtonscott@example.net</t>
+          <t>wilsondavid@example.org</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>964-687-2772x129</t>
+          <t>688-978-3814</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Megan</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Barnett</t>
+          <t>Clark</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>christine17@example.net</t>
+          <t>zmccarthy@example.org</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>501-640-9031x05900</t>
+          <t>253-872-0966</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Evan</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Welch</t>
+          <t>King</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>christopher51@example.net</t>
+          <t>whitneyferguson@example.com</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>(662)780-9440x053</t>
+          <t>932-783-9197x072</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lindsey</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Parker</t>
+          <t>Andrews</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>monica32@example.org</t>
+          <t>thomasoneill@example.org</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>001-787-327-3584x9420</t>
+          <t>+1-783-289-4694x68221</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cervantes</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>sethparker@example.com</t>
+          <t>susanthomas@example.com</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>(799)782-5744x012</t>
+          <t>+1-507-227-3275</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Laura</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>George</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>melaniebenjamin@example.org</t>
+          <t>rosecox@example.com</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>(622)277-4572x964</t>
+          <t>001-632-639-6738</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Marvin</t>
+          <t>Gabriela</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Campbell</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>hsimmons@example.com</t>
+          <t>johnbrown@example.net</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>(778)648-1137x11166</t>
+          <t>+1-375-596-4328x74145</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Abigail</t>
+          <t>Patty</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ochoa</t>
+          <t>Gregory</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>panderson@example.org</t>
+          <t>sheltonphillip@example.com</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>522-303-5795</t>
+          <t>496-302-7768x50249</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Curtis</t>
+          <t>Albert</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>garciatamara@example.org</t>
+          <t>charles87@example.org</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>001-378-580-7051x53127</t>
+          <t>+1-230-864-2679x949</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Jillian</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Lang</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>floresmorgan@example.net</t>
+          <t>garrettkelsey@example.net</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6808536489</t>
+          <t>419.981.6103x4274</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Hannah</t>
+          <t>Nancy</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Perez</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>kerri51@example.com</t>
+          <t>sbrown@example.net</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>+1-410-708-9322x90979</t>
+          <t>+1-568-329-1081x978</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Benson</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>qlewis@example.net</t>
+          <t>danduncan@example.org</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>286-989-3219</t>
+          <t>(934)282-5500</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Kyle</t>
+          <t>Caleb</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Robertson</t>
+          <t>Torres</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>amandabrown@example.com</t>
+          <t>rmccarthy@example.org</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5969562705</t>
+          <t>755.892.7111x981</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Dustin</t>
+          <t>Jenna</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Gonzales</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>perezsandra@example.org</t>
+          <t>ajohnson@example.com</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>736-972-7905</t>
+          <t>(254)512-0559x5347</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Wesley</t>
+          <t>Larry</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Henry</t>
+          <t>Mclaughlin</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ashley95@example.org</t>
+          <t>suttondavid@example.net</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>+1-313-596-1635</t>
+          <t>(994)618-9510x19469</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Donna</t>
+          <t>Shelby</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>vlambert@example.com</t>
+          <t>chad11@example.net</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>001-979-899-8237x7229</t>
+          <t>(782)413-8582</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Pamela</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Castillo</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ccombs@example.com</t>
+          <t>ohoffman@example.org</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7736297786</t>
+          <t>+1-818-595-2652x457</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>William</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Love</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>bettywilson@example.org</t>
+          <t>egraves@example.org</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>001-797-952-6308x725</t>
+          <t>270-272-3681</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Lauren</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Bullock</t>
+          <t>Jimenez</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>nicole43@example.com</t>
+          <t>hutchinsonnicole@example.org</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>672.603.6729</t>
+          <t>001-212-839-8551</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Amy</t>
+          <t>Justin</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Jenkins</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>heidisuarez@example.org</t>
+          <t>ellenferguson@example.net</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>(756)984-6997</t>
+          <t>764.415.3410x62196</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ortiz</t>
+          <t>Long</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>stephaniebrown@example.org</t>
+          <t>schmidtmichelle@example.org</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>(955)753-5982x6261</t>
+          <t>674.921.0391x576</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cooper</t>
+          <t>Harrington</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>nataliewheeler@example.net</t>
+          <t>wmercer@example.net</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>759.478.6756x7445</t>
+          <t>(740)735-3357x46828</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Christina</t>
+          <t>Erica</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Lyons</t>
+          <t>Adams</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>pchristensen@example.com</t>
+          <t>carrie65@example.org</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>+1-223-259-9310x78600</t>
+          <t>429.791.1693</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Douglas</t>
+          <t>Teresa</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Torres</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>brandi19@example.org</t>
+          <t>davidwilson@example.org</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>205.782.5841x29615</t>
+          <t>217-298-8512x66487</t>
         </is>
       </c>
     </row>

</xml_diff>